<commit_message>
RESTful Client, Goole Books API, JSON, Databinding, Drag'n'Drop
</commit_message>
<xml_diff>
--- a/FrameworkVersionen.xlsx
+++ b/FrameworkVersionen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar2\source\repos\ppedvAG\VB_Sommerhausen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E2E61C-204E-4DAC-9F70-A144F53FB38B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DFDC1A-2EC9-4B56-98A1-8EF8C4BC76D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{B1596342-A2E5-4ADE-894A-780BD56A00E9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{B1596342-A2E5-4ADE-894A-780BD56A00E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
   <si>
     <t>.NET</t>
   </si>
@@ -205,23 +205,70 @@
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Farbe</t>
+  </si>
+  <si>
+    <t>Kraftstoffsorte</t>
+  </si>
+  <si>
+    <t>Leistung</t>
+  </si>
+  <si>
+    <t>Anzahl Türen</t>
+  </si>
+  <si>
+    <t>Umweltklasse</t>
+  </si>
+  <si>
+    <t>Innenausstattung</t>
+  </si>
+  <si>
+    <t>Fahren()</t>
+  </si>
+  <si>
+    <t>Hupen()</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>protected</t>
+  </si>
+  <si>
+    <t>friend</t>
+  </si>
+  <si>
+    <t>protected friend</t>
+  </si>
+  <si>
+    <t>VB</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>protected internal</t>
+  </si>
+  <si>
+    <t>internal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -242,6 +289,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -257,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -265,18 +325,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -285,21 +360,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -315,6 +393,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>124704</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1" descr="dotnet-today">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{735D034C-E247-43A4-8920-FDA366E1A71E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4343400" y="236220"/>
+          <a:ext cx="6647424" cy="3581400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -616,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8FDB3F-9250-48C3-B8F4-0C324BB34CD1}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,7 +792,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -656,10 +800,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
@@ -671,16 +815,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
@@ -695,9 +839,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="14" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -708,8 +852,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
@@ -718,8 +862,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
@@ -734,8 +878,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
@@ -745,8 +889,8 @@
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
@@ -761,16 +905,16 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -784,15 +928,15 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -807,36 +951,36 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
       <c r="E17">
         <v>1603</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
       <c r="E18">
         <v>1609</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
       <c r="E19">
         <v>1703</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="2" t="s">
         <v>33</v>
       </c>
@@ -848,8 +992,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="1" t="s">
         <v>35</v>
       </c>
@@ -859,16 +1003,16 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="D22" s="3"/>
       <c r="E22">
         <v>1809</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="4" t="s">
         <v>34</v>
       </c>
@@ -880,7 +1024,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>37</v>
       </c>
       <c r="E24" t="s">
@@ -894,15 +1038,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A320FFDC-FAC6-4961-BEB5-20C9BC457BC7}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,102 +1057,185 @@
     <col min="3" max="3" width="3.77734375" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" customWidth="1"/>
     <col min="5" max="5" width="3.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F14" s="15" t="s">
+      <c r="I13" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F14" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="L15" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="L16" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="L17" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
         <v>57</v>
       </c>
+      <c r="L18" s="14" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I10:I14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>